<commit_message>
added DeepLearning, SVM poly
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58D7D49-E09A-1245-952A-BEA2CD316B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F54472-65B8-0042-9C30-67517CCCE5F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Model</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Rating (%)</t>
   </si>
   <si>
-    <t>Neureal Network</t>
-  </si>
-  <si>
     <t>kNN</t>
   </si>
   <si>
@@ -65,13 +62,22 @@
     <t>SVM radial</t>
   </si>
   <si>
-    <t>svm poly</t>
+    <t>Neureal Network/Deep Learning</t>
+  </si>
+  <si>
+    <t>Neureal Network/Deep Learning 2</t>
+  </si>
+  <si>
+    <t>SVM polynomial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -101,8 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -255,56 +262,71 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$10</c:f>
+              <c:f>Sheet1!$A$4:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>SVM radial</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>SVM polynomial</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>SVM linear</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Logistic Regression</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>kNN</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Decsion Tree</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Neureal Network</c:v>
+                  <c:v>Random Forest Classifier</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Random Forest Classifier</c:v>
+                  <c:v>Neureal Network/Deep Learning</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Neureal Network/Deep Learning 2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>kNN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$10</c:f>
+              <c:f>Sheet1!$B$4:$B$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="General">
                   <c:v>84.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
                   <c:v>85.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3" formatCode="General">
                   <c:v>89.8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4" formatCode="General">
+                  <c:v>91.1</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>91.8</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>92.1</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>93.1</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
                   <c:v>94.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>91.1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>91.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1362,21 +1384,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1389,7 +1411,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>84.9</v>
@@ -1397,26 +1419,26 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>85.3</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="1">
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>89.8</v>
+        <v>85.3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>94.2</v>
+        <v>89.8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1429,25 +1451,39 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>91.8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>91.8</v>
+        <v>92.1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>93.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>94.2</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B10">
-    <sortCondition ref="B4:B10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B12">
+    <sortCondition ref="B4:B12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
add classify rpts to svm, df predct vs actl to DL
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F54472-65B8-0042-9C30-67517CCCE5F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0B33AE-BE1E-124F-9A46-BB958B0383E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -266,13 +266,13 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>SVM polynomial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SVM linear</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>SVM radial</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>SVM polynomial</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>SVM linear</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Logistic Regression</c:v>
@@ -299,33 +299,33 @@
             <c:numRef>
               <c:f>Sheet1!$B$4:$B$12</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>84.9</c:v>
+                <c:pt idx="0" formatCode="0.0">
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>85.3</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
+                  <c:v>85.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>89.8</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="4">
                   <c:v>91.1</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
                   <c:v>91.8</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>92.1</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>93.1</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="8">
                   <c:v>94.2</c:v>
                 </c:pt>
               </c:numCache>
@@ -421,7 +421,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1387,7 +1387,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1411,26 +1411,26 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>84.9</v>
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1">
-        <v>85</v>
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>85.1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>85.3</v>
+        <v>85.2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
include Silicon isotope data, run kNN
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0B33AE-BE1E-124F-9A46-BB958B0383E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F975CFD-9AF5-4344-9A2E-25DDBB1AAB54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Model</t>
   </si>
@@ -62,13 +62,16 @@
     <t>SVM radial</t>
   </si>
   <si>
-    <t>Neureal Network/Deep Learning</t>
+    <t>SVM polynomial</t>
   </si>
   <si>
-    <t>Neureal Network/Deep Learning 2</t>
+    <t>Deep Learning</t>
   </si>
   <si>
-    <t>SVM polynomial</t>
+    <t>CARBON ONLY</t>
+  </si>
+  <si>
+    <t>CARBON and SILICON</t>
   </si>
 </sst>
 </file>
@@ -262,9 +265,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$12</c:f>
+              <c:f>Sheet1!$A$4:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>SVM polynomial</c:v>
                 </c:pt>
@@ -284,12 +287,9 @@
                   <c:v>Random Forest Classifier</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Neureal Network/Deep Learning</c:v>
+                  <c:v>Deep Learning</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Neureal Network/Deep Learning 2</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>kNN</c:v>
                 </c:pt>
               </c:strCache>
@@ -297,10 +297,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$12</c:f>
+              <c:f>Sheet1!$B$4:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="0.0">
                   <c:v>85</c:v>
                 </c:pt>
@@ -320,12 +320,9 @@
                   <c:v>91.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>92.1</c:v>
+                  <c:v>93.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>93.1</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>94.2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1384,10 +1381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1401,6 +1398,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
@@ -1411,7 +1413,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1">
         <v>85</v>
@@ -1459,26 +1461,39 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>92.1</v>
+        <v>93.1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>93.1</v>
+        <v>94.2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>5</v>
       </c>
-      <c r="B12">
-        <v>94.2</v>
+      <c r="B20">
+        <v>94.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Random Forest Classfier carbon silicon
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F975CFD-9AF5-4344-9A2E-25DDBB1AAB54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FFD7A8-3CE9-BE45-9D5B-1DED753233DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Model</t>
   </si>
@@ -1381,10 +1381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1493,7 +1493,15 @@
         <v>5</v>
       </c>
       <c r="B20">
-        <v>94.7</v>
+        <v>94.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>95.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minmaxscalar for all carbon silicon models
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FFD7A8-3CE9-BE45-9D5B-1DED753233DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C626E237-5257-E04D-B3BB-157CFE89CE00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
+    <workbookView xWindow="2320" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,15 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Model</t>
   </si>
   <si>
     <t>Logistic Regression</t>
-  </si>
-  <si>
-    <t>Decsion Tree</t>
   </si>
   <si>
     <t>Random Forest Classifier</t>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>CARBON and SILICON</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
   </si>
 </sst>
 </file>
@@ -281,7 +281,7 @@
                   <c:v>Logistic Regression</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Decsion Tree</c:v>
+                  <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Random Forest Classifier</c:v>
@@ -1381,10 +1381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1395,12 +1395,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1408,12 +1408,12 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>85</v>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>85.1</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>85.2</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>91.1</v>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>91.8</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>93.1</v>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>94.2</v>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1485,23 +1485,39 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B20">
-        <v>94.8</v>
+        <v>87.2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B21">
-        <v>95.1</v>
+        <v>93.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>94.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>95.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates with 2 sets silicon isotopes
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C626E237-5257-E04D-B3BB-157CFE89CE00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76888878-49C3-E249-8230-49D84C1C21B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -1383,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1493,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="B20">
-        <v>87.2</v>
+        <v>88.3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1501,7 +1501,7 @@
         <v>12</v>
       </c>
       <c r="B21">
-        <v>93.2</v>
+        <v>95.1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1509,7 +1509,7 @@
         <v>4</v>
       </c>
       <c r="B22">
-        <v>94.8</v>
+        <v>94.9</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1517,7 +1517,7 @@
         <v>2</v>
       </c>
       <c r="B23">
-        <v>95.2</v>
+        <v>96.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
run models with C, Si, N, and Al isotopes
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76888878-49C3-E249-8230-49D84C1C21B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CC8083-F49E-F040-A3AA-A90474001698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Model</t>
   </si>
@@ -73,6 +73,9 @@
   <si>
     <t>Decision Tree</t>
   </si>
+  <si>
+    <t>C, Si, N, Al</t>
+  </si>
 </sst>
 </file>
 
@@ -81,8 +84,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -110,9 +121,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1381,10 +1393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1399,7 +1411,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1476,7 +1488,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1518,6 +1530,43 @@
       </c>
       <c r="B23">
         <v>96.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>85.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29">
+        <v>93.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>95.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add C N and C Si N to four models
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CC8083-F49E-F040-A3AA-A90474001698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E84B3F7-F049-534D-A461-4CF3C82BB6E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t>Model</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>C, Si, N, Al</t>
+  </si>
+  <si>
+    <t>CARBON and NITROGEN</t>
+  </si>
+  <si>
+    <t>C, Si, N</t>
   </si>
 </sst>
 </file>
@@ -1393,10 +1399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1569,6 +1575,80 @@
         <v>95.1</v>
       </c>
     </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>82.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <v>91.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>90.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>87.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>84.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41">
+        <v>95.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>96.9</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B12">
     <sortCondition ref="B4:B12"/>

</xml_diff>

<commit_message>
added DL carbon silicon nitrogen
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E84B3F7-F049-534D-A461-4CF3C82BB6E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75331B2E-F245-7D47-9F48-4BCF2C63B42D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>Model</t>
   </si>
@@ -127,10 +127,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1399,9 +1400,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="150" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -1581,71 +1582,87 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>1</v>
+      <c r="A33" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B33">
-        <v>82.4</v>
+        <v>80.099999999999994</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B34">
-        <v>91.4</v>
+        <v>82.4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B35">
-        <v>90.7</v>
+        <v>91.4</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>90.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>2</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>95.8</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39">
-        <v>87.1</v>
-      </c>
-    </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>1</v>
+      <c r="A40" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B40">
-        <v>84.4</v>
+        <v>78.2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B41">
-        <v>95.7</v>
+        <v>87.1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>84.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <v>95.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>2</v>
       </c>
-      <c r="B42">
+      <c r="B44">
         <v>96.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added DL carbon silicon nitrogen alum
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75331B2E-F245-7D47-9F48-4BCF2C63B42D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342B9606-8917-0E45-8DA7-E21957EC0A1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>Model</t>
   </si>
@@ -1400,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1539,6 +1539,14 @@
         <v>96.8</v>
       </c>
     </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>87.9</v>
+      </c>
+    </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>13</v>
@@ -1546,123 +1554,131 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B27">
-        <v>85.4</v>
+        <v>76.8</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B28">
-        <v>88.5</v>
+        <v>85.4</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B29">
-        <v>93.9</v>
+        <v>88.5</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <v>93.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>2</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>95.1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>80.099999999999994</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34">
-        <v>82.4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B35">
-        <v>91.4</v>
+        <v>82.4</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B36">
-        <v>90.7</v>
+        <v>91.4</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <v>90.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>2</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>95.8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>78.2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41">
-        <v>87.1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B42">
-        <v>84.4</v>
+        <v>87.1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B43">
-        <v>95.7</v>
+        <v>84.4</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44">
+        <v>95.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>2</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>96.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add models for silicon only
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342B9606-8917-0E45-8DA7-E21957EC0A1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DD0C31-794C-8646-88F9-9BBD193B464C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
   <si>
     <t>Model</t>
   </si>
@@ -82,6 +82,12 @@
   <si>
     <t>C, Si, N</t>
   </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t># records</t>
+  </si>
 </sst>
 </file>
 
@@ -127,11 +133,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1400,10 +1407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1509,18 +1516,18 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>88.3</v>
+        <v>87.9</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B21">
-        <v>95.1</v>
+        <v>88.3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1533,18 +1540,18 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B23">
-        <v>96.8</v>
+        <v>95.1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B24">
-        <v>87.9</v>
+        <v>96.8</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1592,12 +1599,12 @@
         <v>95.1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
@@ -1605,7 +1612,7 @@
         <v>80.099999999999994</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -1613,23 +1620,23 @@
         <v>82.4</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>90.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>12</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>91.4</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37">
-        <v>90.7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -1637,12 +1644,12 @@
         <v>95.8</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>9</v>
       </c>
@@ -1650,23 +1657,23 @@
         <v>78.2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>84.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>4</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>87.1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43">
-        <v>84.4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -1674,7 +1681,7 @@
         <v>95.7</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -1682,9 +1689,68 @@
         <v>96.9</v>
       </c>
     </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="4">
+        <v>14679</v>
+      </c>
+      <c r="D47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48">
+        <v>80.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49">
+        <v>85.6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50">
+        <v>86.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>88.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52">
+        <v>88.7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>89.2</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B12">
-    <sortCondition ref="B4:B12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:B45">
+    <sortCondition ref="B41:B45"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
XGBoost for carbon nitrogen
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DD0C31-794C-8646-88F9-9BBD193B464C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169F579D-39DC-5543-A63C-7042290F5616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
   <si>
     <t>Model</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t># records</t>
+  </si>
+  <si>
+    <t>XGBoost</t>
   </si>
 </sst>
 </file>
@@ -1407,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1603,6 +1606,12 @@
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C33" s="4">
+        <v>2189</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
@@ -1644,113 +1653,121 @@
         <v>95.8</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>78.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42">
-        <v>84.4</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B43">
-        <v>87.1</v>
+        <v>84.4</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B44">
-        <v>95.7</v>
+        <v>87.1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45">
+        <v>95.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>2</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>96.9</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C48" s="4">
         <v>14679</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48">
-        <v>80.8</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B49">
-        <v>85.6</v>
+        <v>80.8</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B50">
-        <v>86.8</v>
+        <v>85.6</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B51">
-        <v>88.1</v>
+        <v>86.8</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B52">
-        <v>88.7</v>
+        <v>88.1</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53">
+        <v>88.7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>4</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>89.2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:B45">
-    <sortCondition ref="B41:B45"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A42:B46">
+    <sortCondition ref="B42:B46"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
add XGBoost carbon silicon nitrogen
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169F579D-39DC-5543-A63C-7042290F5616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3753CB5F-3146-0947-9F0D-860A5434B5DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
   <si>
     <t>Model</t>
   </si>
@@ -1410,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1665,6 +1665,12 @@
       <c r="A41" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="C41" s="4">
+        <v>1301</v>
+      </c>
+      <c r="D41" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
@@ -1700,74 +1706,82 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46">
+        <v>96.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>2</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>96.9</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C49" s="4">
         <v>14679</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>12</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>80.8</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>2</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <v>85.6</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>7</v>
       </c>
-      <c r="B51">
+      <c r="B52">
         <v>86.8</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>1</v>
       </c>
-      <c r="B52">
+      <c r="B53">
         <v>88.1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>9</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>88.7</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>4</v>
       </c>
-      <c r="B54">
+      <c r="B55">
         <v>89.2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A42:B46">
-    <sortCondition ref="B42:B46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A42:B47">
+    <sortCondition ref="B42:B47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
add XGBoost for other element combos
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3753CB5F-3146-0947-9F0D-860A5434B5DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6A8D7C-E5C6-154A-AAD6-B60E03C2AF5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
+    <workbookView xWindow="4640" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
   <si>
     <t>Model</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>kNN</t>
-  </si>
-  <si>
-    <t>Machine Learning Model comparison for Meteorite Classification</t>
   </si>
   <si>
     <t>SVM linear</t>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>XGBoost</t>
+  </si>
+  <si>
+    <t>Machine Learning Model Comparison for Meteorite Classification</t>
   </si>
 </sst>
 </file>
@@ -294,9 +294,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$11</c:f>
+              <c:f>Sheet1!$A$4:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>SVM polynomial</c:v>
                 </c:pt>
@@ -319,6 +319,9 @@
                   <c:v>Deep Learning</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>XGBoost</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>kNN</c:v>
                 </c:pt>
               </c:strCache>
@@ -326,10 +329,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$11</c:f>
+              <c:f>Sheet1!$B$4:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="0.0">
                   <c:v>85</c:v>
                 </c:pt>
@@ -352,6 +355,9 @@
                   <c:v>93.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>93.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>94.2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1084,7 +1090,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1410,10 +1416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1422,17 +1428,23 @@
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4">
+        <v>15622</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1440,31 +1452,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>85.1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>85.2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1472,15 +1484,15 @@
         <v>89.8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>91.1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1488,300 +1500,344 @@
         <v>91.8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>93.1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>93.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>94.2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="4">
+        <v>14423</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>87.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>88.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>94.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20">
-        <v>87.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B24">
+        <v>95.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25">
+        <v>96.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>96.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>328</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>76.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>85.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>1</v>
       </c>
-      <c r="B21">
-        <v>88.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22">
-        <v>94.9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23">
+      <c r="B31">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32">
+        <v>93.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33">
         <v>95.1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>2</v>
       </c>
-      <c r="B24">
-        <v>96.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="B34">
+        <v>95.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27">
-        <v>76.8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28">
-        <v>85.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29">
-        <v>88.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30">
-        <v>93.9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31">
-        <v>95.1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="4">
+      <c r="C36" s="4">
         <v>2189</v>
       </c>
-      <c r="D33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34">
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37">
         <v>80.099999999999994</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35">
-        <v>82.4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36">
-        <v>90.7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37">
-        <v>91.4</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B38">
-        <v>95.8</v>
+        <v>82.4</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B39">
+        <v>90.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40">
+        <v>91.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41">
         <v>95.8</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="4">
         <v>1301</v>
       </c>
-      <c r="D41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42">
+      <c r="D44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
         <v>78.2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43">
-        <v>84.4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44">
-        <v>87.1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45">
-        <v>95.7</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B46">
-        <v>96.3</v>
+        <v>84.4</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B47">
-        <v>96.9</v>
+        <v>87.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48">
+        <v>95.7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="4">
-        <v>14679</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="A49" t="s">
         <v>17</v>
+      </c>
+      <c r="B49">
+        <v>96.3</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B50">
-        <v>80.8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51">
-        <v>85.6</v>
+        <v>96.9</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>7</v>
-      </c>
-      <c r="B52">
-        <v>86.8</v>
+      <c r="A52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="4">
+        <v>14679</v>
+      </c>
+      <c r="D52" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B53">
-        <v>88.1</v>
+        <v>80.8</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B54">
-        <v>88.7</v>
+        <v>85.6</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55">
+        <v>86.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56">
+        <v>87.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>88.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58">
+        <v>88.7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>4</v>
       </c>
-      <c r="B55">
+      <c r="B59">
         <v>89.2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A42:B47">
-    <sortCondition ref="B42:B47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A45:B50">
+    <sortCondition ref="B45:B50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
tried SVM on others, add sheets to xlsx
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788A4998-0A24-1943-910C-4D5E58C35CFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A2439D-45AD-E449-8E16-18AE7C89C7B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="840" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
+    <workbookView xWindow="1380" yWindow="840" windowWidth="23320" windowHeight="16140" firstSheet="2" activeTab="13" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
   <sheets>
     <sheet name="C" sheetId="1" r:id="rId1"/>
@@ -19,20 +19,20 @@
     <sheet name="C Si N" sheetId="5" r:id="rId4"/>
     <sheet name="C Si N Al" sheetId="6" r:id="rId5"/>
     <sheet name="Si" sheetId="7" r:id="rId6"/>
-    <sheet name="RFC" sheetId="9" r:id="rId7"/>
-    <sheet name="XGBoost" sheetId="8" r:id="rId8"/>
+    <sheet name="XGBoost" sheetId="8" r:id="rId7"/>
+    <sheet name="RFC" sheetId="9" r:id="rId8"/>
     <sheet name="Dec.Tree" sheetId="10" r:id="rId9"/>
     <sheet name="kNN" sheetId="13" r:id="rId10"/>
     <sheet name="LogReg" sheetId="12" r:id="rId11"/>
     <sheet name="DeepLearn" sheetId="11" r:id="rId12"/>
+    <sheet name="Model Avg" sheetId="17" r:id="rId13"/>
+    <sheet name="Top 5" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">kNN!$A$4:$A$9</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">kNN!$B$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">kNN!$B$4:$B$9</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">kNN!$A$4:$A$9</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">kNN!$B$3</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">kNN!$B$4:$B$9</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Top 5'!$A$29:$A$43</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Top 5'!$B$29:$B$43</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'Top 5'!$A$29:$A$43</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'Top 5'!$B$29:$B$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="93">
   <si>
     <t>Model</t>
   </si>
@@ -94,24 +94,6 @@
   </si>
   <si>
     <t>Machine Learning Model Comparison for Meteorite Classification</t>
-  </si>
-  <si>
-    <t>Rating (%) Carbon Isotopes</t>
-  </si>
-  <si>
-    <t>Rating (%) Carbon &amp; Silicon Isotopes</t>
-  </si>
-  <si>
-    <t>Rating (%) Carbon &amp; Nitrogen Isotopes</t>
-  </si>
-  <si>
-    <t>Rating (%) Carbon, Silicon, &amp; Nitrogen Isotopes</t>
-  </si>
-  <si>
-    <t>Rating (%) Carbon, Silicon, Nitrogen, &amp; Aluminum Isotopes</t>
-  </si>
-  <si>
-    <t>Rating (%) Silicon Isotopes</t>
   </si>
   <si>
     <t>SILICON (Si)</t>
@@ -156,34 +138,199 @@
     <t>Random Forest Classifier (RFC)</t>
   </si>
   <si>
-    <t>Rating (%) Decision Tree</t>
-  </si>
-  <si>
-    <t>Rating (%) Deep Learning</t>
-  </si>
-  <si>
-    <t>Rating (%) Random Forest Classifier</t>
-  </si>
-  <si>
-    <t>Rating (%) XGBoost</t>
-  </si>
-  <si>
     <t>Logistic Regression (LogReg)</t>
   </si>
   <si>
-    <t>Rating (%) Logistic Regression</t>
-  </si>
-  <si>
     <t>k Nearest Neighbor (kNN)</t>
-  </si>
-  <si>
-    <t>Rating (%) k Nearest Neighbor</t>
   </si>
   <si>
     <t>Decision Tree (Dec.Tree)</t>
   </si>
   <si>
     <t>Deep Learning (DeepLearn)</t>
+  </si>
+  <si>
+    <t>Average Accuracy</t>
+  </si>
+  <si>
+    <t>This shows the model's average accuracy</t>
+  </si>
+  <si>
+    <t>across all combinations of elements,</t>
+  </si>
+  <si>
+    <t>indicating that XGBoost is likely the best</t>
+  </si>
+  <si>
+    <t>model for this set of data as a whole.</t>
+  </si>
+  <si>
+    <t>Model and Elements</t>
+  </si>
+  <si>
+    <t>Accuracy (%)</t>
+  </si>
+  <si>
+    <t>Accuracy (%) Deep Learning</t>
+  </si>
+  <si>
+    <t>Accuracy (%) Logistic Regression</t>
+  </si>
+  <si>
+    <t>Accuracy (%) k Nearest Neighbor</t>
+  </si>
+  <si>
+    <t>Accuracy (%) Decision Tree</t>
+  </si>
+  <si>
+    <t>Accuracy (%) Random Forest Classifier</t>
+  </si>
+  <si>
+    <t>Accuracy (%) XGBoost</t>
+  </si>
+  <si>
+    <t>Accuracy (%) Silicon Isotopes</t>
+  </si>
+  <si>
+    <t>Accuracy (%) Carbon, Silicon, Nitrogen, &amp; Aluminum Isotopes</t>
+  </si>
+  <si>
+    <t>Accuracy (%) Carbon, Silicon, &amp; Nitrogen Isotopes</t>
+  </si>
+  <si>
+    <t>Accuracy (%) Carbon &amp; Nitrogen Isotopes</t>
+  </si>
+  <si>
+    <t>Accuracy (%) Carbon &amp; Silicon Isotopes</t>
+  </si>
+  <si>
+    <t>Accuracy (%) Carbon Isotopes</t>
+  </si>
+  <si>
+    <t>Decision Tree: Si</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier: Si</t>
+  </si>
+  <si>
+    <t>SVM radial: Si</t>
+  </si>
+  <si>
+    <t>XGBoost: Si</t>
+  </si>
+  <si>
+    <t>Logistic Regression: Si</t>
+  </si>
+  <si>
+    <t>Deep Learning: Si</t>
+  </si>
+  <si>
+    <t>kNN: Si</t>
+  </si>
+  <si>
+    <t>SVM linear: C Si N Al</t>
+  </si>
+  <si>
+    <t>Deep Learning: C Si N Al</t>
+  </si>
+  <si>
+    <t>kNN: C Si N Al</t>
+  </si>
+  <si>
+    <t>Logistic Regression: C Si N Al</t>
+  </si>
+  <si>
+    <t>Decision Tree: C Si N Al</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier: C Si N Al</t>
+  </si>
+  <si>
+    <t>XGBoost: C Si N Al</t>
+  </si>
+  <si>
+    <t>SVM radial: C Si N</t>
+  </si>
+  <si>
+    <t>Deep Learning: C Si N</t>
+  </si>
+  <si>
+    <t>Logistic Regression: C Si N</t>
+  </si>
+  <si>
+    <t>kNN: C Si N</t>
+  </si>
+  <si>
+    <t>Decision Tree: C Si N</t>
+  </si>
+  <si>
+    <t>XGBoost: C Si N</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier: C Si N</t>
+  </si>
+  <si>
+    <t>Deep Learning: C N</t>
+  </si>
+  <si>
+    <t>Logistic Regression: C N</t>
+  </si>
+  <si>
+    <t>kNN: C N</t>
+  </si>
+  <si>
+    <t>Decision Tree: C N</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier: C N</t>
+  </si>
+  <si>
+    <t>XGBoost: C N</t>
+  </si>
+  <si>
+    <t>Deep Learning: C Si</t>
+  </si>
+  <si>
+    <t>Logistic Regression: C Si</t>
+  </si>
+  <si>
+    <t>kNN: C Si</t>
+  </si>
+  <si>
+    <t>Decision Tree: C Si</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier: C Si</t>
+  </si>
+  <si>
+    <t>XGBoost: C Si</t>
+  </si>
+  <si>
+    <t>SVM polynomial: C</t>
+  </si>
+  <si>
+    <t>SVM linear: C</t>
+  </si>
+  <si>
+    <t>SVM radial: C</t>
+  </si>
+  <si>
+    <t>Logistic Regression: C</t>
+  </si>
+  <si>
+    <t>Decision Tree: C</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier: C</t>
+  </si>
+  <si>
+    <t>Deep Learning: C</t>
+  </si>
+  <si>
+    <t>XGBoost: C</t>
+  </si>
+  <si>
+    <t>kNN: C</t>
   </si>
 </sst>
 </file>
@@ -237,10 +384,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -319,7 +466,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rating (%) Carbon Isotopes</c:v>
+                  <c:v>Accuracy (%) Carbon Isotopes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -693,7 +840,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rating (%) k Nearest Neighbor</c:v>
+                  <c:v>Accuracy (%) k Nearest Neighbor</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1048,7 +1195,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rating (%) Logistic Regression</c:v>
+                  <c:v>Accuracy (%) Logistic Regression</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1346,7 +1493,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rating (%) Deep Learning</c:v>
+                  <c:v>Accuracy (%) Deep Learning</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1641,6 +1788,724 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Model Avg'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Model Avg'!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Deep Learning</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>kNN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random Forest Classifier</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>XGBoost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Model Avg'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>84.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>86.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9C3C-6840-BE9D-15CAF63458C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1887343712"/>
+        <c:axId val="1887345344"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1887343712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1887345344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1887345344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1887343712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Top 5 Model and Elements Combinations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Top 5'!$A$39:$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>XGBoost: C N</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>XGBoost: C Si N</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Forest Classifier: C Si</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>XGBoost: C Si</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random Forest Classifier: C Si N</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Top 5'!$B$39:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>95.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-44A8-6349-A854-9CBA4C2BE855}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="184452831"/>
+        <c:axId val="184344591"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="184452831"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="184344591"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="184344591"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="184452831"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -1701,7 +2566,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rating (%) Carbon &amp; Silicon Isotopes</c:v>
+                  <c:v>Accuracy (%) Carbon &amp; Silicon Isotopes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1791,10 +2656,10 @@
                   <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Random Forest Classifier</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>XGBoost</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Random Forest Classifier</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2056,7 +2921,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rating (%) Carbon &amp; Nitrogen Isotopes</c:v>
+                  <c:v>Accuracy (%) Carbon &amp; Nitrogen Isotopes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2146,10 +3011,10 @@
                   <c:v>Decision Tree</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Random Forest Classifier</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>XGBoost</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Random Forest Classifier</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2411,7 +3276,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rating (%) Carbon, Silicon, &amp; Nitrogen Isotopes</c:v>
+                  <c:v>Accuracy (%) Carbon, Silicon, &amp; Nitrogen Isotopes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2485,25 +3350,28 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'C Si N'!$A$5:$A$10</c:f>
+              <c:f>'C Si N'!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>SVM radial</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Deep Learning</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Logistic Regression</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>kNN</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Decision Tree</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>XGBoost</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Random Forest Classifier</c:v>
                 </c:pt>
               </c:strCache>
@@ -2511,26 +3379,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'C Si N'!$B$5:$B$10</c:f>
+              <c:f>'C Si N'!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>72.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>78.2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>84.4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>87.1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>95.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>96.3</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>96.9</c:v>
                 </c:pt>
               </c:numCache>
@@ -2766,7 +3637,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rating (%) Carbon, Silicon, Nitrogen, &amp; Aluminum Isotopes</c:v>
+                  <c:v>Accuracy (%) Carbon, Silicon, Nitrogen, &amp; Aluminum Isotopes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2840,52 +3711,58 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'C Si N Al'!$A$5:$A$10</c:f>
+              <c:f>'C Si N Al'!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>SVM linear</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Deep Learning</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>kNN</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Logistic Regression</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Decision Tree</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>XGBoost</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Random Forest Classifier</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>XGBoost</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'C Si N Al'!$B$5:$B$10</c:f>
+              <c:f>'C Si N Al'!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>68.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>76.8</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>85.4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>88.5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>93.9</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>95.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>95.1</c:v>
                 </c:pt>
               </c:numCache>
@@ -3121,7 +3998,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rating (%) Silicon Isotopes</c:v>
+                  <c:v>Accuracy (%) Silicon Isotopes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3478,11 +4355,366 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>XGBoost!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy (%) XGBoost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>XGBoost!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Si</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C Si N Al</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>C N</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>C Si N</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>C Si</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>XGBoost!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>87.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-77B4-B542-9A13-B48116EBBD8F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="202576495"/>
+        <c:axId val="1886817776"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="202576495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1886817776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1886817776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="202576495"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>RFC!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rating (%) Random Forest Classifier</c:v>
+                  <c:v>Accuracy (%) Random Forest Classifier</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3720,361 +4952,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>XGBoost!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Rating (%) XGBoost</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>XGBoost!$A$4:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Si</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>C</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>C Si N Al</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>C N</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>C Si N</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>C Si</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>XGBoost!$B$4:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>87.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>93.7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>95.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>95.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>96.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>96.8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-77B4-B542-9A13-B48116EBBD8F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="202576495"/>
-        <c:axId val="1886817776"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="202576495"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1886817776"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1886817776"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="202576495"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -4135,7 +5012,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rating (%) Decision Tree</c:v>
+                  <c:v>Accuracy (%) Decision Tree</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4551,6 +5428,86 @@
 </file>
 
 <file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6930,6 +7887,1016 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -11016,15 +12983,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
+      <xdr:colOff>474133</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>63499</xdr:rowOff>
+      <xdr:rowOff>71966</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>702733</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>67733</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>165099</xdr:rowOff>
+      <xdr:rowOff>173566</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11057,15 +13024,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>262467</xdr:colOff>
+      <xdr:colOff>448734</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>46567</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>42334</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>148167</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11097,16 +13064,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>821266</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>135467</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>414866</xdr:colOff>
+      <xdr:colOff>558800</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11114,6 +13081,88 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFE724BD-CA90-B94A-B402-3F3437983987}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>84667</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>21166</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>122766</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F705B44-1362-3144-A89D-88BED0595569}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD15F9BA-132E-8342-8BCC-B0A68B93FEE7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11343,16 +13392,57 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>12699</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8226EAE0-4EB1-244D-A999-C6071F41547F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>601133</xdr:colOff>
+      <xdr:colOff>778933</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>8466</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>194733</xdr:colOff>
+      <xdr:colOff>372533</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>110066</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11380,61 +13470,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>440267</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>80433</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>33867</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>182033</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8226EAE0-4EB1-244D-A999-C6071F41547F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>745066</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>93133</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>148166</xdr:rowOff>
+      <xdr:rowOff>29632</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>338666</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>46566</xdr:rowOff>
+      <xdr:colOff>516466</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>131232</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11761,8 +13810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11778,9 +13827,9 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -11794,7 +13843,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -11890,27 +13939,27 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>85.4</v>
@@ -11918,7 +13967,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>87.1</v>
@@ -11928,13 +13977,13 @@
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>89.2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>90.7</v>
@@ -11942,7 +13991,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>94.2</v>
@@ -11950,7 +13999,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>94.9</v>
@@ -11958,7 +14007,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
         <f>AVERAGE(B4:B9)</f>
@@ -11979,27 +14028,27 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>39</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>82.4</v>
@@ -12007,7 +14056,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>84.4</v>
@@ -12017,13 +14066,13 @@
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>88.1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>88.3</v>
@@ -12031,7 +14080,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>88.5</v>
@@ -12039,7 +14088,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>89.8</v>
@@ -12047,7 +14096,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
         <f>AVERAGE(B4:B9)</f>
@@ -12068,27 +14117,27 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>35</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>76.8</v>
@@ -12096,7 +14145,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>78.2</v>
@@ -12104,7 +14153,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>80.099999999999994</v>
@@ -12112,7 +14161,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>87.9</v>
@@ -12122,13 +14171,13 @@
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>88.7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>93.1</v>
@@ -12136,7 +14185,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
         <f>AVERAGE(B4:B9)</f>
@@ -12146,6 +14195,466 @@
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B9">
     <sortCondition ref="B4:B9"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4E6F9C-BEE9-4345-9758-F7DEB184279D}">
+  <dimension ref="A2:B13"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>84.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>86.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>90.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>91.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>93.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>94.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5758CE-B4DA-0249-8C3B-79FDAC094704}">
+  <dimension ref="A1:B43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>68.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>76.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>78.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6">
+        <v>80.099999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7">
+        <v>80.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8">
+        <v>82.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9">
+        <v>84.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11">
+        <v>85.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13">
+        <v>85.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14">
+        <v>85.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15">
+        <v>86.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16">
+        <v>87.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17">
+        <v>87.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18">
+        <v>87.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19">
+        <v>88.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20">
+        <v>88.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22">
+        <v>88.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23">
+        <v>89.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24">
+        <v>89.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25">
+        <v>90.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26">
+        <v>91.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27">
+        <v>91.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28">
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29">
+        <v>93.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30">
+        <v>93.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31">
+        <v>93.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32">
+        <v>94.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33">
+        <v>94.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34">
+        <v>95.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35">
+        <v>95.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36">
+        <v>95.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37">
+        <v>95.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40">
+        <v>96.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41">
+        <v>96.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42">
+        <v>96.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43">
+        <v>96.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B43">
+    <sortCondition ref="B2:B43"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12157,7 +14666,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12167,9 +14676,9 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -12183,7 +14692,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -12220,7 +14729,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>96.8</v>
@@ -12228,7 +14737,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>96.8</v>
@@ -12246,7 +14755,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12256,9 +14765,9 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -12272,7 +14781,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -12309,7 +14818,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>95.8</v>
@@ -12317,7 +14826,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>95.8</v>
@@ -12331,10 +14840,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D41E1F4D-6E04-774A-8F26-25B82AEB54F9}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12344,9 +14853,9 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -12361,55 +14870,63 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>78.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>84.4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>87.1</v>
+        <v>84.4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>95.7</v>
+        <v>87.1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>96.3</v>
+        <v>95.7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>96.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>96.9</v>
       </c>
     </row>
@@ -12421,10 +14938,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9AB3D5-238C-6D41-925F-2667132DD098}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12435,9 +14952,9 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -12454,47 +14971,47 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>76.8</v>
+        <v>68.3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>85.4</v>
+        <v>76.8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>88.5</v>
+        <v>85.4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>93.9</v>
+        <v>88.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>95.1</v>
+        <v>93.9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -12502,6 +15019,14 @@
         <v>2</v>
       </c>
       <c r="B10">
+        <v>95.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
         <v>95.1</v>
       </c>
     </row>
@@ -12516,7 +15041,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12526,9 +15051,9 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -12542,7 +15067,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -12609,95 +15134,6 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730C9984-54F3-6D4A-A83B-45E7D9232264}">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="6">
-        <v>85.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5">
-        <v>91.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6">
-        <v>95.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7">
-        <v>95.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8">
-        <v>96.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9">
-        <v>96.9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="1">
-        <f>AVERAGE(B5:B9)</f>
-        <v>95.28</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B9">
-    <sortCondition ref="B4:B9"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A7B97-D620-664D-AF52-0FC1C32658AF}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -12714,23 +15150,23 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>87.8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>93.7</v>
@@ -12738,7 +15174,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>95.1</v>
@@ -12746,7 +15182,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>95.8</v>
@@ -12754,7 +15190,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>96.3</v>
@@ -12762,7 +15198,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>96.8</v>
@@ -12770,7 +15206,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
         <f>AVERAGE(B4:B9)</f>
@@ -12780,6 +15216,95 @@
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B9">
     <sortCondition ref="B6:B9"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730C9984-54F3-6D4A-A83B-45E7D9232264}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5">
+        <v>85.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>95.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>96.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>96.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1">
+        <f>AVERAGE(B4:B9)</f>
+        <v>93.666666666666671</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B9">
+    <sortCondition ref="B4:B9"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12791,35 +15316,35 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>80.8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>91.1</v>
@@ -12827,7 +15352,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>91.4</v>
@@ -12835,7 +15360,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>93.9</v>
@@ -12843,7 +15368,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>95.1</v>
@@ -12851,7 +15376,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>95.7</v>
@@ -12859,7 +15384,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
         <f>AVERAGE(B4:B9)</f>

</xml_diff>

<commit_message>
add Excel files for Tableau
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A2439D-45AD-E449-8E16-18AE7C89C7B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC8D690-5A22-8248-AE4F-78E8995A3831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="840" windowWidth="23320" windowHeight="16140" firstSheet="2" activeTab="13" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -29,10 +29,10 @@
     <sheet name="Top 5" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Top 5'!$A$29:$A$43</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Top 5'!$B$29:$B$43</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'Top 5'!$A$29:$A$43</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'Top 5'!$B$29:$B$43</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Top 5'!$B$29:$B$43</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Top 5'!$C$29:$C$43</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'Top 5'!$B$29:$B$43</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'Top 5'!$C$29:$C$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="93">
   <si>
     <t>Model</t>
   </si>
@@ -2291,7 +2291,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Top 5'!$A$39:$A$43</c:f>
+              <c:f>'Top 5'!$B$39:$B$43</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2314,7 +2314,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Top 5'!$B$39:$B$43</c:f>
+              <c:f>'Top 5'!$C$39:$C$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -13146,13 +13146,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -14299,362 +14299,492 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5758CE-B4DA-0249-8C3B-79FDAC094704}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>68.3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>65</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>72.400000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>59</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>76.8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>78.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>80.099999999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>80.8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>73</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>82.4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>67</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>84.4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
         <v>85</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>85.1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
         <v>86</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>85.2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
         <v>60</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>85.4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
         <v>52</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>85.6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
         <v>53</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>86.8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
         <v>68</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>87.1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
         <v>54</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>87.8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
         <v>78</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>87.9</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
         <v>55</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>88.1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
         <v>79</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>88.3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
         <v>61</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>88.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
         <v>56</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>88.7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
         <v>57</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>89.2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
         <v>87</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>89.8</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
         <v>74</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>90.7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
         <v>88</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>91.1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
         <v>75</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>91.4</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
         <v>89</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>91.8</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
         <v>90</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>93.1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
         <v>91</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>93.7</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
         <v>62</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>93.9</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
         <v>92</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>94.2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
         <v>80</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>94.9</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
         <v>63</v>
       </c>
-      <c r="B34">
+      <c r="C34">
         <v>95.1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s">
         <v>64</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>95.1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
         <v>81</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>95.1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
         <v>69</v>
       </c>
-      <c r="B37">
+      <c r="C37">
         <v>95.7</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
         <v>76</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>95.8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
         <v>77</v>
       </c>
-      <c r="B39">
+      <c r="C39">
         <v>95.8</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
         <v>70</v>
       </c>
-      <c r="B40">
+      <c r="C40">
         <v>96.3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
         <v>82</v>
       </c>
-      <c r="B41">
+      <c r="C41">
         <v>96.8</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" t="s">
         <v>83</v>
       </c>
-      <c r="B42">
+      <c r="C42">
         <v>96.8</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
         <v>71</v>
       </c>
-      <c r="B43">
+      <c r="C43">
         <v>96.9</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B43">
-    <sortCondition ref="B2:B43"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C43">
+    <sortCondition ref="C2:C43"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
feature imporance and other tests
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED59F271-9E9C-E64E-BFDB-D6EC68239AF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83866C8-6AAA-BF4B-A0A9-B84EFAA05E92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="460" windowWidth="23320" windowHeight="16140" firstSheet="2" activeTab="13" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
+    <workbookView xWindow="4880" yWindow="460" windowWidth="23320" windowHeight="15940" firstSheet="4" activeTab="14" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
   <sheets>
     <sheet name="C" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,12 @@
     <sheet name="DeepLearn" sheetId="11" r:id="rId12"/>
     <sheet name="Model Avg" sheetId="17" r:id="rId13"/>
     <sheet name="Top 5" sheetId="14" r:id="rId14"/>
+    <sheet name="feature importance" sheetId="18" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Top 5'!$B$29:$B$43</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Top 5'!$C$29:$C$43</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'Top 5'!$B$29:$B$43</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'Top 5'!$C$29:$C$43</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">'feature importance'!$A$4:$A$7</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'feature importance'!$B$3</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'feature importance'!$B$4:$B$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="100">
   <si>
     <t>Model</t>
   </si>
@@ -332,6 +332,27 @@
   <si>
     <t>kNN: C</t>
   </si>
+  <si>
+    <t>Random Forest Classifer C Si N feature importances</t>
+  </si>
+  <si>
+    <t>carbon 12 13</t>
+  </si>
+  <si>
+    <t>nitrogen 14 15</t>
+  </si>
+  <si>
+    <t>silicon 29 28</t>
+  </si>
+  <si>
+    <t>silicon 30 28</t>
+  </si>
+  <si>
+    <t>elemental isotopes</t>
+  </si>
+  <si>
+    <t>contribution (%)</t>
+  </si>
 </sst>
 </file>
 
@@ -365,7 +386,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -373,11 +394,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -389,6 +419,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2464,6 +2495,292 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="184452831"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'feature importance'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>contribution (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'feature importance'!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>nitrogen 14 15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>silicon 29 28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>silicon 30 28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>carbon 12 13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'feature importance'!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-769B-8B47-B915-A0A5EA8103CC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1040157215"/>
+        <c:axId val="969665391"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1040157215"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="969665391"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="969665391"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1040157215"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5553,6 +5870,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -8903,6 +9260,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -13169,6 +14031,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD15F9BA-132E-8342-8BCC-B0A68B93FEE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9094684-661E-DC45-BAA0-4768CCAD8BC5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14305,7 +15208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5758CE-B4DA-0249-8C3B-79FDAC094704}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -14797,12 +15700,86 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D4A192-5AEA-7B45-A92D-9735BBD62F33}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="1">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="1">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="1">
+        <v>47.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="7">
+        <f>SUM(B4:B7)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B7">
+    <sortCondition ref="B4:B7"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3F2FE0-6F54-944F-BD57-4EDDEF7D932D}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
prediction analysis on XGBoost C Si
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83866C8-6AAA-BF4B-A0A9-B84EFAA05E92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0361BE8-C045-D648-89DC-67258552B767}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="460" windowWidth="23320" windowHeight="15940" firstSheet="4" activeTab="14" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
+    <workbookView xWindow="4860" yWindow="460" windowWidth="23320" windowHeight="15940" firstSheet="4" activeTab="14" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
   <sheets>
     <sheet name="C" sheetId="1" r:id="rId1"/>
@@ -2618,6 +2618,63 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'feature importance'!$A$4:$A$7</c:f>

</xml_diff>

<commit_message>
feature contributions in excel
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0361BE8-C045-D648-89DC-67258552B767}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E2CD4D-385A-F145-B186-8D70677439A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="460" windowWidth="23320" windowHeight="15940" firstSheet="4" activeTab="14" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
+    <workbookView xWindow="4860" yWindow="460" windowWidth="23320" windowHeight="15940" firstSheet="5" activeTab="15" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
   <sheets>
     <sheet name="C" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,14 @@
     <sheet name="LogReg" sheetId="12" r:id="rId11"/>
     <sheet name="DeepLearn" sheetId="11" r:id="rId12"/>
     <sheet name="Model Avg" sheetId="17" r:id="rId13"/>
-    <sheet name="Top 5" sheetId="14" r:id="rId14"/>
+    <sheet name="Top 6" sheetId="14" r:id="rId14"/>
     <sheet name="feature importance" sheetId="18" r:id="rId15"/>
+    <sheet name="# records" sheetId="19" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">'feature importance'!$A$4:$A$7</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'feature importance'!$B$3</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'feature importance'!$B$4:$B$7</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">'# records'!$A$3:$A$5</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'# records'!$B$2</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'# records'!$B$3:$B$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="102">
   <si>
     <t>Model</t>
   </si>
@@ -352,6 +353,12 @@
   </si>
   <si>
     <t>contribution (%)</t>
+  </si>
+  <si>
+    <t>isotope</t>
+  </si>
+  <si>
+    <t>combinations</t>
   </si>
 </sst>
 </file>
@@ -2322,7 +2329,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Top 5'!$B$38:$B$43</c:f>
+              <c:f>'Top 6'!$B$38:$B$43</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2348,7 +2355,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Top 5'!$C$38:$C$43</c:f>
+              <c:f>'Top 6'!$C$38:$C$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2838,6 +2845,343 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1040157215"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'# records'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># records</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'# records'!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>C Si N</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>C N</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C Si</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'# records'!$B$3:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2189</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="#,##0">
+                  <c:v>14423</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6C4F-8042-8858-C311452C05E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1044293967"/>
+        <c:axId val="1044295599"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1044293967"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1044295599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1044295599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1044293967"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5967,6 +6311,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -9822,6 +10206,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -14129,6 +15018,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9094684-661E-DC45-BAA0-4768CCAD8BC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>29633</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>524933</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>131233</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA7EF3E6-571C-364C-91F1-3273F60849FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15266,7 +16196,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15761,7 +16691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D4A192-5AEA-7B45-A92D-9735BBD62F33}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -15825,6 +16755,65 @@
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B7">
     <sortCondition ref="B4:B7"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D2F542-EA78-7A48-8EEF-9535F4611863}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4">
+        <v>14423</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B5">
+    <sortCondition ref="B3:B5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
add feature importance, conf. matrix top 6
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E2CD4D-385A-F145-B186-8D70677439A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCDDF07-16F6-9E4E-9719-62659983DE78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="460" windowWidth="23320" windowHeight="15940" firstSheet="5" activeTab="15" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
+    <workbookView xWindow="4820" yWindow="480" windowWidth="23320" windowHeight="15940" firstSheet="7" activeTab="15" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
   <sheets>
     <sheet name="C" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,14 @@
     <sheet name="DeepLearn" sheetId="11" r:id="rId12"/>
     <sheet name="Model Avg" sheetId="17" r:id="rId13"/>
     <sheet name="Top 6" sheetId="14" r:id="rId14"/>
-    <sheet name="feature importance" sheetId="18" r:id="rId15"/>
-    <sheet name="# records" sheetId="19" r:id="rId16"/>
+    <sheet name="feature importance RFC C Si N" sheetId="18" r:id="rId15"/>
+    <sheet name="feature importance RFC C Si" sheetId="20" r:id="rId16"/>
+    <sheet name="# records" sheetId="19" r:id="rId17"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">'# records'!$A$3:$A$5</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'# records'!$B$2</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'# records'!$B$3:$B$5</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">'feature importance RFC C Si'!$A$4:$A$6</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'feature importance RFC C Si'!$B$3</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'feature importance RFC C Si'!$B$4:$B$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="108">
   <si>
     <t>Model</t>
   </si>
@@ -360,6 +361,24 @@
   <si>
     <t>combinations</t>
   </si>
+  <si>
+    <t>Random Forest Classifer C Si feature importances</t>
+  </si>
+  <si>
+    <t>Run RFC C Si 10 times</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Run RFC C Si N 10 times</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
 </sst>
 </file>
 
@@ -414,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -427,6 +446,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2342,13 +2362,13 @@
                   <c:v>XGBoost: C Si N</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>XGBoost: C Si</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Random Forest Classifier: C Si N</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Random Forest Classifier: C Si</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>XGBoost: C Si</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Random Forest Classifier: C Si N</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2372,10 +2392,10 @@
                   <c:v>96.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96.8</c:v>
+                  <c:v>96.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>96.9</c:v>
+                  <c:v>97.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2606,7 +2626,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'feature importance'!$B$3</c:f>
+              <c:f>'feature importance RFC C Si N'!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2684,7 +2704,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'feature importance'!$A$4:$A$7</c:f>
+              <c:f>'feature importance RFC C Si N'!$A$4:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2704,7 +2724,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'feature importance'!$B$4:$B$7</c:f>
+              <c:f>'feature importance RFC C Si N'!$B$4:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2894,6 +2914,343 @@
 </file>
 
 <file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'feature importance RFC C Si'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>contribution (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'feature importance RFC C Si'!$A$4:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>silicon 30 28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>silicon 29 28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>carbon 12 13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'feature importance RFC C Si'!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>19.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7C04-894F-8730-ABA236699DB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1074976831"/>
+        <c:axId val="971620351"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1074976831"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="971620351"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="971620351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1074976831"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6351,6 +6708,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -10711,6 +11108,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -15039,6 +15941,47 @@
 </file>
 
 <file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>198967</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>728133</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>97367</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFD141D4-C695-EB41-B377-9EF1EB1931DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -16195,8 +17138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5758CE-B4DA-0249-8C3B-79FDAC094704}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="A27" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16647,10 +17590,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C41">
         <v>96.8</v>
@@ -16658,13 +17601,13 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C42">
-        <v>96.8</v>
+        <v>96.9</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -16672,15 +17615,15 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C43">
-        <v>96.9</v>
+        <v>97.3</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C43">
-    <sortCondition ref="C2:C43"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C42">
+    <sortCondition ref="C2:C42"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16689,7 +17632,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D4A192-5AEA-7B45-A92D-9735BBD62F33}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -16697,8 +17640,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -16750,6 +17693,80 @@
       <c r="B8" s="7">
         <f>SUM(B4:B7)</f>
         <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>96.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>96.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>96.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>96.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>96.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>96.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>96.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>96.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>96.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>97.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="8">
+        <f>AVERAGE(B17:B26)</f>
+        <v>96.86999999999999</v>
+      </c>
+      <c r="C27">
+        <f>MEDIAN(B17:B26)</f>
+        <v>96.9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -16762,10 +17779,204 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5463F5F7-192A-CD4F-B054-839FFA707B86}">
+  <dimension ref="A1:K30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30:K30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="1">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="1">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="1">
+        <v>58.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="7">
+        <f>SUM(B4:B6)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>97.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>97.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>97.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>97.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>97.3</v>
+      </c>
+      <c r="H20" t="s">
+        <v>107</v>
+      </c>
+      <c r="I20">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>97.3</v>
+      </c>
+      <c r="I21">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>97.2</v>
+      </c>
+      <c r="I22">
+        <v>95.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>97.3</v>
+      </c>
+      <c r="I23">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>97.3</v>
+      </c>
+      <c r="I24">
+        <v>95.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>97.3</v>
+      </c>
+      <c r="I25">
+        <v>95.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="8">
+        <f>AVERAGE(B16:B25)</f>
+        <v>97.309999999999988</v>
+      </c>
+      <c r="C26">
+        <f>MEDIAN(B16:B25)</f>
+        <v>97.3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>105</v>
+      </c>
+      <c r="I26">
+        <v>95.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I28">
+        <v>95.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I29">
+        <v>95.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" s="8">
+        <f>AVERAGE(I20:I29)</f>
+        <v>95.68</v>
+      </c>
+      <c r="J30">
+        <f>MEDIAN(I20:I29)</f>
+        <v>95.6</v>
+      </c>
+      <c r="K30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B6">
+    <sortCondition ref="B4:B6"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D2F542-EA78-7A48-8EEF-9535F4611863}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
put files into folder so README is visible
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/meteorite-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0D1496-96AE-EC4E-9D98-9ED3543D1F8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208B4D57-D48D-9247-B996-E206D31C8109}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="940" windowWidth="23320" windowHeight="15940" activeTab="11" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
+    <workbookView xWindow="4580" yWindow="760" windowWidth="23320" windowHeight="15940" firstSheet="18" activeTab="20" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
   <sheets>
     <sheet name="C" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,23 @@
     <sheet name="kNN" sheetId="13" r:id="rId10"/>
     <sheet name="LogReg" sheetId="12" r:id="rId11"/>
     <sheet name="DeepLearn" sheetId="11" r:id="rId12"/>
-    <sheet name="Model Avg" sheetId="17" r:id="rId13"/>
-    <sheet name="Top 6" sheetId="14" r:id="rId14"/>
-    <sheet name="# records" sheetId="19" r:id="rId15"/>
-    <sheet name="feature importance RFC C Si N" sheetId="18" r:id="rId16"/>
-    <sheet name="feature importance RFC C Si" sheetId="20" r:id="rId17"/>
-    <sheet name="feature imp. XGBoost C Si N" sheetId="21" r:id="rId18"/>
+    <sheet name="SVM" sheetId="24" r:id="rId13"/>
+    <sheet name="Model Avg" sheetId="17" r:id="rId14"/>
+    <sheet name="Top 6" sheetId="14" r:id="rId15"/>
+    <sheet name="# records for top 6" sheetId="19" r:id="rId16"/>
+    <sheet name="total # records" sheetId="22" r:id="rId17"/>
+    <sheet name="feature importance RFC C Si N" sheetId="18" r:id="rId18"/>
+    <sheet name="feature importance RFC C Si" sheetId="20" r:id="rId19"/>
+    <sheet name="feature imp. XGBoost C Si N" sheetId="21" r:id="rId20"/>
+    <sheet name="feature imp. XGBoost C Si" sheetId="23" r:id="rId21"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">SVM!$A$4:$A$8</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">SVM!$B$3</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">SVM!$B$4:$B$8</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">SVM!$C$3</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">SVM!$C$4:$C$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -50,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="120">
   <si>
     <t>Model</t>
   </si>
@@ -346,9 +356,6 @@
     <t>silicon 30 28</t>
   </si>
   <si>
-    <t>elemental isotopes</t>
-  </si>
-  <si>
     <t>contribution (%)</t>
   </si>
   <si>
@@ -378,6 +385,42 @@
   <si>
     <t>Run RFC C N 10 times</t>
   </si>
+  <si>
+    <t>isotope combinations</t>
+  </si>
+  <si>
+    <t>records</t>
+  </si>
+  <si>
+    <t>XGBoost C Si feature importances</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>C polynomial</t>
+  </si>
+  <si>
+    <t>C radial</t>
+  </si>
+  <si>
+    <t>C linear</t>
+  </si>
+  <si>
+    <t>C Si N radial</t>
+  </si>
+  <si>
+    <t>C Si N Al linear</t>
+  </si>
+  <si>
+    <t>isotopes</t>
+  </si>
+  <si>
+    <t>Isotopes</t>
+  </si>
+  <si>
+    <t>Contribution (%)</t>
+  </si>
 </sst>
 </file>
 
@@ -386,7 +429,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -398,6 +441,21 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -432,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -446,6 +504,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1917,6 +1978,472 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SVM Model:</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Accuracy (%)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SVM!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>SVM!$A$4:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>C Si N Al linear</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>C Si N radial</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C polynomial</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>C linear</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>C radial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SVM!$B$4:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>68.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.0">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B33-8E4E-B09F-6DCE6753E20B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1045237295"/>
+        <c:axId val="1045238927"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>SVM!$C$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>SVM!$A$4:$A$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>C Si N Al linear</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>C Si N radial</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>C polynomial</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>C linear</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>C radial</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>SVM!$C$4:$C$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-5B33-8E4E-B09F-6DCE6753E20B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1045237295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1045238927"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1045238927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1045237295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2257,7 +2784,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2626,7 +3153,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2682,7 +3209,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'# records'!$B$2</c:f>
+              <c:f>'# records for top 6'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2760,7 +3287,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'# records'!$A$3:$A$5</c:f>
+              <c:f>'# records for top 6'!$A$3:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2777,7 +3304,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'# records'!$B$3:$B$5</c:f>
+              <c:f>'# records for top 6'!$B$3:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2963,7 +3490,403 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> records by isotope</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> combinations</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'total # records'!$B$1:$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>isotope</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>records</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'total # records'!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>C Si N Al</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>C Si N</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C N</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>C Si</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Si</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'total # records'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1301</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2189</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0">
+                  <c:v>14423</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="#,##0">
+                  <c:v>14679</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="#,##0">
+                  <c:v>15622</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9C85-6746-B4C4-92F20456F942}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="982488079"/>
+        <c:axId val="1074184095"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="982488079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1074184095"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1074184095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="982488079"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3339,7 +4262,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3432,7 +4355,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>contribution (%)</c:v>
+                  <c:v>Contribution (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3709,7 +4632,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3765,11 +4688,391 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>'C Si'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy (%) Carbon &amp; Silicon Isotopes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'C Si'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Deep Learning</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>kNN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>XGBoost</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Random Forest Classifier</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'C Si'!$B$5:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>87.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-385B-2841-A528-D2E790E45659}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="181670559"/>
+        <c:axId val="196270639"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="181670559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="196270639"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="196270639"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="181670559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Feature Importance for XGBoost with C Si N contribution (%)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>'feature imp. XGBoost C Si N'!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>contribution (%)</c:v>
+                  <c:v>Contribution (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4052,7 +5355,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4067,6 +5370,39 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Feature Importance for XGBoost</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> with C Si </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>contribution (%)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4108,11 +5444,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'C Si'!$B$4</c:f>
+              <c:f>'feature imp. XGBoost C Si'!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Accuracy (%) Carbon &amp; Silicon Isotopes</c:v>
+                  <c:v>Contribution (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4186,60 +5522,42 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'C Si'!$A$5:$A$10</c:f>
+              <c:f>'feature imp. XGBoost C Si'!$A$4:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Deep Learning</c:v>
+                  <c:v>silicon 29 28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Logistic Regression</c:v>
+                  <c:v>silicon 30 28</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>kNN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Decision Tree</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>XGBoost</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Random Forest Classifier</c:v>
+                  <c:v>carbon 12 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'C Si'!$B$5:$B$10</c:f>
+              <c:f>'feature imp. XGBoost C Si'!$B$4:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>87.9</c:v>
+                  <c:v>17.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88.3</c:v>
+                  <c:v>30.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>94.9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>95.1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>96.8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>97.3</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-385B-2841-A528-D2E790E45659}"/>
+              <c16:uniqueId val="{00000000-BE28-0049-89E0-5C74FFC89A70}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4252,11 +5570,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="181670559"/>
-        <c:axId val="196270639"/>
+        <c:axId val="965542703"/>
+        <c:axId val="986973231"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="181670559"/>
+        <c:axId val="965542703"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4299,7 +5617,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196270639"/>
+        <c:crossAx val="986973231"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4307,7 +5625,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196270639"/>
+        <c:axId val="986973231"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4327,7 +5645,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4358,7 +5676,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="181670559"/>
+        <c:crossAx val="965542703"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7310,7 +8628,127 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors20.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors21.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -12680,7 +14118,1522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style20.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style21.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16889,6 +19842,47 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>641350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{250CA81E-15BC-8844-81EF-82FFF5B6D789}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>84667</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>21166</xdr:rowOff>
@@ -16925,7 +19919,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -16966,7 +19960,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -17007,7 +20001,48 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49B00EC6-41EE-394B-9FA1-5A3DADF7C2E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -17048,7 +20083,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -17069,47 +20104,6 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFD141D4-C695-EB41-B377-9EF1EB1931DF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>753533</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D3BFA48-4F54-0949-86DD-9C11E80F16D7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17151,6 +20145,88 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DAA2E1F-4340-2C40-B99B-22E402CBBA6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>702733</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>186266</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D3BFA48-4F54-0949-86DD-9C11E80F16D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>690034</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BC4E0F3-ADCC-A544-A6A5-49FC753956B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17758,7 +20834,7 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18063,7 +21139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3AA0BEC-C2DA-9043-8F01-8879DDF64468}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -18149,6 +21225,78 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{880E4AA3-7699-3943-AAE5-CB06BBAFCF6B}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4">
+        <v>68.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5">
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7">
+        <v>85.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8">
+        <v>85.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B8">
+    <sortCondition ref="B4:B8"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4E6F9C-BEE9-4345-9758-F7DEB184279D}">
   <dimension ref="A2:B13"/>
   <sheetViews>
@@ -18244,7 +21392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5758CE-B4DA-0249-8C3B-79FDAC094704}">
   <dimension ref="A1:C43"/>
   <sheetViews>
@@ -18740,12 +21888,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D2F542-EA78-7A48-8EEF-9535F4611863}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18755,12 +21903,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -18799,12 +21947,91 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320DE240-BE22-EB4C-B311-8142205E9210}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="9">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="11">
+        <v>14423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>14679</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="4">
+        <v>15622</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D4A192-5AEA-7B45-A92D-9735BBD62F33}">
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18820,10 +22047,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -18866,10 +22093,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -18935,7 +22162,7 @@
         <v>96.9</v>
       </c>
       <c r="D27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -18947,12 +22174,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5463F5F7-192A-CD4F-B054-839FFA707B86}">
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18962,15 +22189,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -19005,10 +22232,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -19031,7 +22258,7 @@
         <v>97.3</v>
       </c>
       <c r="H19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -19095,7 +22322,7 @@
         <v>97.3</v>
       </c>
       <c r="D26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I26">
         <v>95.6</v>
@@ -19129,85 +22356,12 @@
         <v>95.6</v>
       </c>
       <c r="K30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B6">
     <sortCondition ref="B4:B6"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{965305D8-0830-3547-9CF5-314B80032108}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="1">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="1">
-        <v>21.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="1">
-        <v>35.200000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="1">
-        <v>37.799999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B8" s="7">
-        <f>SUM(B4:B7)</f>
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B7">
-    <sortCondition ref="B4:B7"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19303,6 +22457,144 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{965305D8-0830-3547-9CF5-314B80032108}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1">
+        <v>21.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="1">
+        <v>35.200000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="1">
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="7">
+        <f>SUM(B4:B7)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B7">
+    <sortCondition ref="B4:B7"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485F747A-B21B-E74A-B113-2793D34FD729}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="1">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="1">
+        <v>30.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="1">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="7">
+        <f>SUM(B4:B6)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B6">
+    <sortCondition ref="B4:B6"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82756D25-530B-8947-93C4-78F35D7259EF}">
   <dimension ref="A1:C10"/>
@@ -19396,7 +22688,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19494,7 +22786,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>